<commit_message>
adding 3 more projects
</commit_message>
<xml_diff>
--- a/Analysis Results/AnalysisSummary.xlsx
+++ b/Analysis Results/AnalysisSummary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="15000" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>APV</t>
   </si>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,81 +741,61 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>21684</v>
+        <v>1582</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F16">
-        <v>421</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>1582</v>
+        <v>30168</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>1048</v>
       </c>
       <c r="E17">
-        <v>7</v>
+        <v>904</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>30168</v>
+        <v>21183</v>
       </c>
       <c r="C18">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>1048</v>
+        <v>10</v>
       </c>
       <c r="E18">
-        <v>904</v>
+        <v>11</v>
       </c>
       <c r="F18">
-        <v>1626</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <v>21183</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>10</v>
-      </c>
-      <c r="E19">
-        <v>11</v>
-      </c>
-      <c r="F19">
         <v>409</v>
       </c>
     </row>
@@ -824,7 +804,7 @@
     <sortCondition ref="A2:A19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updating results to be actually correct... (stupid bugs...)
</commit_message>
<xml_diff>
--- a/Analysis Results/AnalysisSummary.xlsx
+++ b/Analysis Results/AnalysisSummary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="15000" windowHeight="7755"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="15000" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>APV</t>
   </si>
@@ -33,9 +33,6 @@
     <t>All Source Callees</t>
   </si>
   <si>
-    <t>All Source RCG</t>
-  </si>
-  <si>
     <t>AndroidsFortune</t>
   </si>
   <si>
@@ -85,6 +82,33 @@
   </si>
   <si>
     <t>StoryMaker</t>
+  </si>
+  <si>
+    <t>Secrets</t>
+  </si>
+  <si>
+    <t>WebSMS</t>
+  </si>
+  <si>
+    <t>RemoteDroid</t>
+  </si>
+  <si>
+    <t>Analysis Time (milli-seconds)</t>
+  </si>
+  <si>
+    <t>All Source RCG Nodes</t>
+  </si>
+  <si>
+    <t>All Source RCG Edges</t>
+  </si>
+  <si>
+    <t>Barcode Scanner</t>
+  </si>
+  <si>
+    <t>TRAQ</t>
+  </si>
+  <si>
+    <t>Gcache</t>
   </si>
 </sst>
 </file>
@@ -423,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,10 +460,12 @@
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -447,59 +473,77 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>5003</v>
+      </c>
+      <c r="C2">
+        <v>2906</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>5279</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
       <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>36</v>
+      </c>
+      <c r="H2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
       </c>
       <c r="B3">
         <v>18201</v>
       </c>
       <c r="C3">
+        <v>6454</v>
+      </c>
+      <c r="D3">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>962</v>
-      </c>
       <c r="E3">
-        <v>904</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>175</v>
+      </c>
+      <c r="H3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -507,301 +551,538 @@
         <v>3801</v>
       </c>
       <c r="C4">
+        <v>2797</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>961</v>
-      </c>
       <c r="E4">
-        <v>906</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>33307</v>
       </c>
       <c r="C5">
+        <v>3692</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="D5">
-        <v>1020</v>
-      </c>
       <c r="E5">
-        <v>904</v>
+        <v>70</v>
       </c>
       <c r="F5">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G5">
+        <v>445</v>
+      </c>
+      <c r="H5">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1062</v>
       </c>
       <c r="C6">
+        <v>2733</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>956</v>
-      </c>
       <c r="E6">
-        <v>904</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>9725</v>
       </c>
       <c r="C7">
+        <v>3196</v>
+      </c>
+      <c r="D7">
         <v>16</v>
       </c>
-      <c r="D7">
-        <v>978</v>
-      </c>
       <c r="E7">
-        <v>908</v>
+        <v>35</v>
       </c>
       <c r="F7">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <v>171</v>
+      </c>
+      <c r="H7">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1564</v>
       </c>
       <c r="C8">
+        <v>2845</v>
+      </c>
+      <c r="D8">
         <v>11</v>
       </c>
-      <c r="D8">
-        <v>963</v>
-      </c>
       <c r="E8">
-        <v>904</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G8">
+        <v>63</v>
+      </c>
+      <c r="H8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>51518</v>
       </c>
       <c r="C9">
+        <v>4727</v>
+      </c>
+      <c r="D9">
         <v>9</v>
       </c>
-      <c r="D9">
-        <v>93</v>
-      </c>
       <c r="E9">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="F9">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G9">
+        <v>1158</v>
+      </c>
+      <c r="H9">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>485</v>
       </c>
       <c r="C10">
+        <v>2697</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="D10">
-        <v>961</v>
-      </c>
       <c r="E10">
-        <v>909</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>3201</v>
       </c>
       <c r="C11">
+        <v>2887</v>
+      </c>
+      <c r="D11">
         <v>15</v>
       </c>
-      <c r="D11">
-        <v>963</v>
-      </c>
       <c r="E11">
-        <v>909</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>49047</v>
       </c>
       <c r="C12">
+        <v>6441</v>
+      </c>
+      <c r="D12">
         <v>14</v>
       </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
       <c r="E12">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="F12">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G12">
+        <v>1012</v>
+      </c>
+      <c r="H12">
+        <v>3315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>968</v>
       </c>
       <c r="C13">
+        <v>2887</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
-      <c r="D13">
-        <v>964</v>
-      </c>
       <c r="E13">
-        <v>909</v>
+        <v>4</v>
       </c>
       <c r="F13">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <v>24</v>
+      </c>
+      <c r="H13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>209</v>
       </c>
       <c r="C14">
+        <v>2798</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
-      <c r="D14">
-        <v>962</v>
-      </c>
       <c r="E14">
-        <v>909</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>21684</v>
       </c>
       <c r="C15">
+        <v>3415</v>
+      </c>
+      <c r="D15">
         <v>1</v>
       </c>
-      <c r="D15">
-        <v>10</v>
-      </c>
       <c r="E15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F15">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>512</v>
+      </c>
+      <c r="H15">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>1582</v>
       </c>
       <c r="C16">
+        <v>2952</v>
+      </c>
+      <c r="D16">
         <v>5</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
       </c>
       <c r="E16">
         <v>7</v>
       </c>
       <c r="F16">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="G16">
+        <v>24</v>
+      </c>
+      <c r="H16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B17">
-        <v>30168</v>
+        <v>2819</v>
       </c>
       <c r="C17">
-        <v>17</v>
+        <v>2790</v>
       </c>
       <c r="D17">
-        <v>1048</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>904</v>
+        <v>4</v>
       </c>
       <c r="F17">
-        <v>1626</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>42</v>
+      </c>
+      <c r="H17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18">
+        <v>3350</v>
+      </c>
+      <c r="C18">
+        <v>4416</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>19</v>
+      </c>
+      <c r="G18">
+        <v>51</v>
+      </c>
+      <c r="H18">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>30168</v>
+      </c>
+      <c r="C19">
+        <v>5713</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>136</v>
+      </c>
+      <c r="F19">
+        <v>66</v>
+      </c>
+      <c r="G19">
+        <v>748</v>
+      </c>
+      <c r="H19">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
         <v>21183</v>
       </c>
-      <c r="C18">
+      <c r="C20">
+        <v>4099</v>
+      </c>
+      <c r="D20">
         <v>4</v>
       </c>
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18">
+      <c r="E20">
+        <v>136</v>
+      </c>
+      <c r="F20">
+        <v>66</v>
+      </c>
+      <c r="G20">
+        <v>748</v>
+      </c>
+      <c r="H20">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>24362</v>
+      </c>
+      <c r="C21">
+        <v>3705</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>13</v>
+      </c>
+      <c r="F21">
         <v>11</v>
       </c>
-      <c r="F18">
-        <v>409</v>
+      <c r="G21">
+        <v>525</v>
+      </c>
+      <c r="H21">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>6307</v>
+      </c>
+      <c r="C23">
+        <v>5012</v>
+      </c>
+      <c r="E23">
+        <v>33</v>
+      </c>
+      <c r="F23">
+        <v>48</v>
+      </c>
+      <c r="G23">
+        <v>94</v>
+      </c>
+      <c r="H23">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>6094</v>
+      </c>
+      <c r="C24">
+        <v>11123</v>
+      </c>
+      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <v>15</v>
+      </c>
+      <c r="G24">
+        <v>56</v>
+      </c>
+      <c r="H24">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>54909</v>
+      </c>
+      <c r="C25">
+        <v>5357</v>
+      </c>
+      <c r="E25">
+        <v>293</v>
+      </c>
+      <c r="F25">
+        <v>204</v>
+      </c>
+      <c r="G25">
+        <v>1058</v>
+      </c>
+      <c r="H25">
+        <v>2191</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:XFD19">
-    <sortCondition ref="A2:A19"/>
+  <sortState ref="A2:F21">
+    <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>